<commit_message>
Atualização do código e novos arquivos
</commit_message>
<xml_diff>
--- a/machine-learning/results/metrics.xlsx
+++ b/machine-learning/results/metrics.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -497,10 +497,10 @@
         <v>99.62</v>
       </c>
       <c r="G2" t="n">
-        <v>98.84999999999999</v>
+        <v>99.62</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="3">
@@ -513,16 +513,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>99.62</v>
+        <v>100</v>
       </c>
       <c r="D3" t="n">
-        <v>0.38</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>99.62</v>
+        <v>100</v>
       </c>
       <c r="G3" t="n">
         <v>99.23</v>
@@ -553,10 +553,10 @@
         <v>99.62</v>
       </c>
       <c r="G4" t="n">
-        <v>99.62</v>
+        <v>98.84999999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>0.77</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="5">
@@ -569,22 +569,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>99.23</v>
+        <v>100</v>
       </c>
       <c r="D5" t="n">
-        <v>0.77</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>99.23</v>
+        <v>100</v>
       </c>
       <c r="G5" t="n">
         <v>98.08</v>
       </c>
       <c r="H5" t="n">
-        <v>2.11</v>
+        <v>1.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Descrição do que foi alterado
</commit_message>
<xml_diff>
--- a/machine-learning/results/metrics.xlsx
+++ b/machine-learning/results/metrics.xlsx
@@ -497,10 +497,10 @@
         <v>99.62</v>
       </c>
       <c r="G2" t="n">
-        <v>99.62</v>
+        <v>98.84999999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>0.77</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -541,22 +541,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>99.62</v>
+        <v>100</v>
       </c>
       <c r="D4" t="n">
-        <v>0.38</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>99.62</v>
+        <v>100</v>
       </c>
       <c r="G4" t="n">
-        <v>98.84999999999999</v>
+        <v>98.45999999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>1.54</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="5">
@@ -569,22 +569,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>100</v>
+        <v>99.62</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="F5" t="n">
-        <v>100</v>
+        <v>99.62</v>
       </c>
       <c r="G5" t="n">
-        <v>98.08</v>
+        <v>99.23</v>
       </c>
       <c r="H5" t="n">
-        <v>1.22</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>